<commit_message>
[web] - System variable [`nexial.screenshotAsDesktop`]: *NEW* System variable to allow for desktop screen capturing instead of browser-scoped screen capturing.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_web.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_web.data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10804"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2DD731-0E20-3E44-BA5E-0618F49CE839}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C26D8B-1B38-D24F-A652-58A6C52C77BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>true</t>
   </si>
   <si>
-    <t>800</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>Test Automation</t>
+  </si>
+  <si>
+    <t>600</t>
   </si>
 </sst>
 </file>
@@ -631,7 +631,7 @@
   <dimension ref="A1:AAA200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -644,10 +644,10 @@
   <sheetData>
     <row r="1" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="GQ1" s="4"/>
       <c r="HA1" s="3"/>
@@ -656,10 +656,10 @@
     </row>
     <row r="2" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="GQ2" s="4"/>
       <c r="HA2" s="3"/>
@@ -668,7 +668,7 @@
     </row>
     <row r="3" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>0</v>
@@ -680,10 +680,10 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="GQ4" s="4"/>
       <c r="HA4" s="6"/>
@@ -692,7 +692,7 @@
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>0</v>
@@ -705,10 +705,10 @@
     </row>
     <row r="6" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="GQ6" s="4"/>
       <c r="HA6" s="6"/>
@@ -717,7 +717,7 @@
     </row>
     <row r="7" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>0</v>
@@ -729,26 +729,26 @@
     </row>
     <row r="8" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="HA8" s="6"/>
       <c r="AAA8" s="7"/>
     </row>
     <row r="9" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="C9" s="4"/>
       <c r="E9" s="4"/>
@@ -758,10 +758,10 @@
     </row>
     <row r="10" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="GQ10" s="4"/>
       <c r="HA10" s="6"/>
@@ -770,10 +770,10 @@
     </row>
     <row r="11" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="GQ11" s="4"/>
       <c r="ZQ11" s="4"/>

</xml_diff>

<commit_message>
[localdb] - [`importCSV(var,csv,table)`]: code fix to support columns with spaces or commas
[web]
- [`saveDivsAsCsv(headers,rows,cells,nextPage,file)`]: support non-XPATH locators.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_web.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_web.data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9027576C-6054-8943-AAD4-A09624C9AEB2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA22D09-2049-5A4E-AB87-448333C6FE7B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="10500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -740,10 +740,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>14</v>

</xml_diff>